<commit_message>
sertifikat, surat pernyataan, logo, fitur pencarian nama
</commit_message>
<xml_diff>
--- a/file_import_data/dataPesertaSudahBisaMengambilSertifikat.xlsx
+++ b/file_import_data/dataPesertaSudahBisaMengambilSertifikat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\toeic\file_import_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C93A788B-5FCD-413D-8192-F7E072F26669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62180AA2-FA15-45FC-8004-7D8CC08EC6A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{825CB76D-AFB2-4DE5-A041-44892E4336A4}"/>
   </bookViews>
@@ -45,10 +45,10 @@
     <t>Ismi Atika</t>
   </si>
   <si>
-    <t>Aqila Nur Azza</t>
+    <t>No.</t>
   </si>
   <si>
-    <t>No.</t>
+    <t>Kemal S</t>
   </si>
 </sst>
 </file>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,7 +424,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -449,10 +449,10 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>2341760022</v>
+        <v>2341760196</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>